<commit_message>
Updated script and template.
Updated script and template to adjust the row high
to the content of the questions and the options.
</commit_message>
<xml_diff>
--- a/domande_risposte.xlsx
+++ b/domande_risposte.xlsx
@@ -346,56 +346,80 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -524,182 +548,183 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="14.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -721,457 +746,527 @@
   </sheetPr>
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="3.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="3.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="3.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="3.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="3.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="3.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="3.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="3.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="17.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="10.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="H5" s="2" t="s">
+      <c r="B5" s="11"/>
+      <c r="H5" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+    <row r="7" s="14" customFormat="true" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="13" t="s">
         <v>56</v>
       </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="3.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" s="11" customFormat="true" ht="38.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+    <row r="9" s="16" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="6.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+    <row r="10" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" s="14" customFormat="true" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="13" t="s">
         <v>56</v>
       </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="3.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" s="11" customFormat="true" ht="38.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+    <row r="13" s="16" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="6.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+    <row r="14" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" s="14" customFormat="true" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="13" t="s">
         <v>56</v>
       </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="3.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" s="11" customFormat="true" ht="38.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
+    <row r="17" s="16" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="6.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+    <row r="18" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" s="14" customFormat="true" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="13" t="s">
         <v>56</v>
       </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="3.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" s="11" customFormat="true" ht="38.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
+    <row r="21" s="16" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="6.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+    <row r="22" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" s="14" customFormat="true" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="13" t="s">
         <v>56</v>
       </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="3.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" s="11" customFormat="true" ht="38.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
+    <row r="25" s="16" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="6.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+    <row r="26" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="27" s="14" customFormat="true" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="13" t="s">
         <v>56</v>
       </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="3.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" s="11" customFormat="true" ht="38.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
+    <row r="29" s="16" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="6.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+    <row r="30" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" s="14" customFormat="true" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="13" t="s">
         <v>56</v>
       </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="3.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" s="11" customFormat="true" ht="38.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10" t="s">
+    <row r="33" s="16" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="H33" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="6.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
+    <row r="34" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" s="14" customFormat="true" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="13" t="s">
         <v>56</v>
       </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="3.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="37" s="11" customFormat="true" ht="38.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="s">
+    <row r="37" s="16" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G37" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="H37" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="6.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="2" t="s">
+    <row r="38" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" s="14" customFormat="true" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="13" t="s">
         <v>56</v>
       </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="3.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="41" s="11" customFormat="true" ht="38.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="s">
+    <row r="41" s="16" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="G41" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H41" s="11" t="s">
+      <c r="H41" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="6.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="2" t="s">
+    <row r="42" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" s="14" customFormat="true" ht="25.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="13" t="s">
         <v>56</v>
       </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
     </row>
     <row r="44" customFormat="false" ht="3.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="45" s="11" customFormat="true" ht="38.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="10" t="s">
+    <row r="45" s="16" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="G45" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H45" s="11" t="s">
+      <c r="H45" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" s="11" customFormat="true" ht="5.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="G46" s="10"/>
+    <row r="46" s="17" customFormat="true" ht="5.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="G46" s="12"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="15">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B43:H43"/>
     <mergeCell ref="A47:H47"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>